<commit_message>
IDBR outperform more effectively
</commit_message>
<xml_diff>
--- a/IDBR/excel/resuilt_verify.xlsx
+++ b/IDBR/excel/resuilt_verify.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\IDBR\IRDBR\IDBR\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFDFF6E-7EA4-428E-A813-C66899E83C35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D5647F-B657-40AD-82F5-F8D31DBE941C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-960" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{A13DA03A-EA5C-411C-8535-D1B579D97496}"/>
   </bookViews>
@@ -305,6 +305,12 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -313,12 +319,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9243,10 +9243,10 @@
       <c r="D11" t="s">
         <v>29</v>
       </c>
-      <c r="J11" s="19" t="s">
+      <c r="J11" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="20"/>
+      <c r="K11" s="22"/>
       <c r="L11" t="s">
         <v>12</v>
       </c>
@@ -9282,10 +9282,10 @@
       <c r="H12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="18" t="s">
+      <c r="J12" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="18"/>
+      <c r="K12" s="20"/>
       <c r="L12" s="10" t="s">
         <v>4</v>
       </c>
@@ -9876,10 +9876,10 @@
       <c r="H23" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="18" t="s">
+      <c r="J23" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="K23" s="18"/>
+      <c r="K23" s="20"/>
       <c r="L23" s="10" t="s">
         <v>4</v>
       </c>
@@ -10404,10 +10404,10 @@
       <c r="H34" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J34" s="18" t="s">
+      <c r="J34" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K34" s="18"/>
+      <c r="K34" s="20"/>
       <c r="L34" s="10" t="s">
         <v>4</v>
       </c>
@@ -10882,10 +10882,10 @@
       <c r="H45" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J45" s="18" t="s">
+      <c r="J45" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="K45" s="18"/>
+      <c r="K45" s="20"/>
       <c r="L45" s="10" t="s">
         <v>4</v>
       </c>
@@ -11491,10 +11491,10 @@
       <c r="H56" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J56" s="18" t="s">
+      <c r="J56" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="K56" s="18"/>
+      <c r="K56" s="20"/>
       <c r="L56" s="10" t="s">
         <v>4</v>
       </c>
@@ -11938,10 +11938,10 @@
       <c r="H67" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J67" s="18" t="s">
+      <c r="J67" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K67" s="18"/>
+      <c r="K67" s="20"/>
       <c r="L67" s="10" t="s">
         <v>4</v>
       </c>
@@ -13222,10 +13222,10 @@
       <c r="D11" t="s">
         <v>29</v>
       </c>
-      <c r="J11" s="19" t="s">
+      <c r="J11" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="20"/>
+      <c r="K11" s="22"/>
       <c r="L11" t="s">
         <v>12</v>
       </c>
@@ -13261,10 +13261,10 @@
       <c r="H12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="18" t="s">
+      <c r="J12" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="18"/>
+      <c r="K12" s="20"/>
       <c r="L12" s="10" t="s">
         <v>39</v>
       </c>
@@ -13780,10 +13780,10 @@
       <c r="H23" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="18" t="s">
+      <c r="J23" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="K23" s="18"/>
+      <c r="K23" s="20"/>
       <c r="L23" s="10" t="s">
         <v>39</v>
       </c>
@@ -14202,10 +14202,10 @@
       <c r="H34" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J34" s="18" t="s">
+      <c r="J34" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K34" s="18"/>
+      <c r="K34" s="20"/>
       <c r="L34" s="10" t="s">
         <v>39</v>
       </c>
@@ -14543,10 +14543,10 @@
       <c r="H45" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J45" s="18" t="s">
+      <c r="J45" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="K45" s="18"/>
+      <c r="K45" s="20"/>
       <c r="L45" s="10" t="s">
         <v>39</v>
       </c>
@@ -14872,10 +14872,10 @@
       <c r="H56" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J56" s="18" t="s">
+      <c r="J56" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="K56" s="18"/>
+      <c r="K56" s="20"/>
       <c r="L56" s="10" t="s">
         <v>39</v>
       </c>
@@ -15187,10 +15187,10 @@
       <c r="H67" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J67" s="18" t="s">
+      <c r="J67" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K67" s="18"/>
+      <c r="K67" s="20"/>
       <c r="L67" s="10" t="s">
         <v>39</v>
       </c>
@@ -20987,10 +20987,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC5236E-3BC3-4DDA-9C36-963E583DCE32}">
-  <dimension ref="A1:AA84"/>
+  <dimension ref="A1:AD84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E43" workbookViewId="0">
-      <selection activeCell="N59" sqref="N59:W61"/>
+    <sheetView tabSelected="1" topLeftCell="E28" workbookViewId="0">
+      <selection activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21004,9 +21004,17 @@
     <col min="9" max="9" width="12.5703125" customWidth="1"/>
     <col min="10" max="10" width="19.42578125" customWidth="1"/>
     <col min="11" max="11" width="18.7109375" customWidth="1"/>
+    <col min="21" max="21" width="15.140625" customWidth="1"/>
+    <col min="22" max="22" width="13.42578125" customWidth="1"/>
+    <col min="23" max="23" width="11.85546875" customWidth="1"/>
+    <col min="24" max="24" width="12.7109375" customWidth="1"/>
+    <col min="25" max="25" width="13.85546875" customWidth="1"/>
+    <col min="26" max="26" width="11.5703125" customWidth="1"/>
+    <col min="28" max="28" width="12.7109375" customWidth="1"/>
+    <col min="29" max="29" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -21020,7 +21028,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -21034,7 +21042,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -21048,7 +21056,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -21056,7 +21064,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -21064,12 +21072,12 @@
         <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -21077,7 +21085,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -21085,7 +21093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -21093,7 +21101,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>44</v>
       </c>
@@ -21107,7 +21115,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -21117,10 +21125,10 @@
       <c r="C13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="18" t="s">
         <v>45</v>
       </c>
       <c r="G13" s="4" t="s">
@@ -21132,10 +21140,10 @@
       <c r="I13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="21" t="s">
+      <c r="J13" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="K13" s="21" t="s">
+      <c r="K13" s="18" t="s">
         <v>45</v>
       </c>
       <c r="N13" s="15">
@@ -21156,8 +21164,38 @@
       <c r="S13">
         <v>5.8524299999999996E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U13" s="15">
+        <v>48810300</v>
+      </c>
+      <c r="V13" s="15">
+        <v>43801500</v>
+      </c>
+      <c r="W13" s="2">
+        <f>(V13-U13)/U13</f>
+        <v>-0.10261768520168899</v>
+      </c>
+      <c r="X13" s="15">
+        <v>48810300</v>
+      </c>
+      <c r="Y13" s="15">
+        <v>35751500</v>
+      </c>
+      <c r="Z13" s="2">
+        <f>(Y13-X13)/X13</f>
+        <v>-0.26754189177284304</v>
+      </c>
+      <c r="AB13" s="15">
+        <v>43801500</v>
+      </c>
+      <c r="AC13" s="15">
+        <v>35751500</v>
+      </c>
+      <c r="AD13" s="2">
+        <f>(AC13-AB13)/AB13</f>
+        <v>-0.18378366037692773</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>0.01</v>
       </c>
@@ -21200,8 +21238,38 @@
       <c r="S14">
         <v>9.5994099999999992E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U14" s="15">
+        <v>52748900</v>
+      </c>
+      <c r="V14" s="15">
+        <v>46830500</v>
+      </c>
+      <c r="W14" s="2">
+        <f t="shared" ref="W14:W16" si="0">(V14-U14)/U14</f>
+        <v>-0.11219949610323628</v>
+      </c>
+      <c r="X14" s="15">
+        <v>52748900</v>
+      </c>
+      <c r="Y14" s="15">
+        <v>39512600</v>
+      </c>
+      <c r="Z14" s="2">
+        <f t="shared" ref="Z14:Z16" si="1">(Y14-X14)/X14</f>
+        <v>-0.25093035115424206</v>
+      </c>
+      <c r="AB14" s="15">
+        <v>46830500</v>
+      </c>
+      <c r="AC14" s="15">
+        <v>39512600</v>
+      </c>
+      <c r="AD14" s="2">
+        <f t="shared" ref="AD14:AD16" si="2">(AC14-AB14)/AB14</f>
+        <v>-0.15626354619318605</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>0.02</v>
       </c>
@@ -21244,8 +21312,38 @@
       <c r="S15">
         <v>1.7141300000000002E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U15" s="15">
+        <v>59959500</v>
+      </c>
+      <c r="V15" s="15">
+        <v>51608300</v>
+      </c>
+      <c r="W15" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.139280681126427</v>
+      </c>
+      <c r="X15" s="15">
+        <v>59959500</v>
+      </c>
+      <c r="Y15" s="15">
+        <v>45949700</v>
+      </c>
+      <c r="Z15" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.23365438337544508</v>
+      </c>
+      <c r="AB15" s="15">
+        <v>51608300</v>
+      </c>
+      <c r="AC15" s="15">
+        <v>45949700</v>
+      </c>
+      <c r="AD15" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.10964515397717034</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>0.03</v>
       </c>
@@ -21288,8 +21386,38 @@
       <c r="S16">
         <v>2.71852E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U16" s="6">
+        <v>61426900</v>
+      </c>
+      <c r="V16" s="6">
+        <v>52562400</v>
+      </c>
+      <c r="W16" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.14430974052084672</v>
+      </c>
+      <c r="X16" s="6">
+        <v>61426900</v>
+      </c>
+      <c r="Y16" s="6">
+        <v>47583300</v>
+      </c>
+      <c r="Z16" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.22536706231309084</v>
+      </c>
+      <c r="AB16" s="6">
+        <v>52562400</v>
+      </c>
+      <c r="AC16" s="6">
+        <v>47583300</v>
+      </c>
+      <c r="AD16" s="2">
+        <f t="shared" si="2"/>
+        <v>-9.4727409707319299E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>0.04</v>
       </c>
@@ -21332,8 +21460,20 @@
       <c r="S17">
         <v>3.4696999999999999E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="W17" s="2">
+        <f>AVERAGE(W13:W16)</f>
+        <v>-0.12460190073804975</v>
+      </c>
+      <c r="Z17" s="2">
+        <f>AVERAGE(Z13:Z16)</f>
+        <v>-0.24437342215390528</v>
+      </c>
+      <c r="AD17" s="2">
+        <f>AVERAGE(AD13:AD16)</f>
+        <v>-0.13610494256365085</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>0.05</v>
       </c>
@@ -21377,7 +21517,7 @@
         <v>4.6983499999999997E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>0.1</v>
       </c>
@@ -21420,8 +21560,18 @@
       <c r="S19">
         <v>7.6358800000000004E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U19">
+        <v>167.29</v>
+      </c>
+      <c r="V19">
+        <v>148.476</v>
+      </c>
+      <c r="W19" s="2">
+        <f t="shared" ref="W19:W22" si="3">(V19-U19)/U19</f>
+        <v>-0.11246338693287103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B20" s="5">
         <v>0.5</v>
       </c>
@@ -21464,8 +21614,18 @@
       <c r="S20">
         <v>8.3452799999999994E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U20" s="12">
+        <v>0.29509600000000002</v>
+      </c>
+      <c r="V20" s="12">
+        <v>0.47873199999999999</v>
+      </c>
+      <c r="W20" s="2">
+        <f t="shared" si="3"/>
+        <v>0.62229240653888884</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B21" s="5">
         <v>1</v>
       </c>
@@ -21508,8 +21668,18 @@
       <c r="S21">
         <v>9.1664300000000004E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U21">
+        <v>7.42004E-2</v>
+      </c>
+      <c r="V21">
+        <v>9.3226699999999996E-2</v>
+      </c>
+      <c r="W21" s="2">
+        <f t="shared" si="3"/>
+        <v>0.25641775516034948</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B22" s="5">
         <v>5</v>
       </c>
@@ -21552,8 +21722,18 @@
       <c r="S22">
         <v>9.3226699999999996E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U22" s="6">
+        <v>819.74374999999998</v>
+      </c>
+      <c r="V22">
+        <v>788.60500000000002</v>
+      </c>
+      <c r="W22" s="2">
+        <f t="shared" si="3"/>
+        <v>-3.7985955977096454E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B23" s="5">
         <v>10</v>
       </c>
@@ -21579,7 +21759,7 @@
         <v>47583300</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>22</v>
       </c>
@@ -21589,10 +21769,10 @@
       <c r="C25" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="D25" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="E25" s="18" t="s">
         <v>43</v>
       </c>
       <c r="F25" s="5"/>
@@ -21605,10 +21785,10 @@
       <c r="I25" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="21" t="s">
+      <c r="J25" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="K25" s="21" t="s">
+      <c r="K25" s="18" t="s">
         <v>45</v>
       </c>
       <c r="N25">
@@ -21626,7 +21806,7 @@
         <v>163.3175</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>0.01</v>
       </c>
@@ -21658,15 +21838,15 @@
         <v>1763.87</v>
       </c>
       <c r="P26">
-        <f t="shared" ref="P26:P34" si="0">N26/8</f>
+        <f t="shared" ref="P26:P34" si="4">N26/8</f>
         <v>1019.3975</v>
       </c>
       <c r="Q26">
-        <f t="shared" ref="Q26:Q34" si="1">O26/8</f>
+        <f t="shared" ref="Q26:Q34" si="5">O26/8</f>
         <v>220.48374999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>0.02</v>
       </c>
@@ -21698,15 +21878,15 @@
         <v>2434.73</v>
       </c>
       <c r="P27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1010.83</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>304.34125</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>0.03</v>
       </c>
@@ -21738,15 +21918,15 @@
         <v>3194.99</v>
       </c>
       <c r="P28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1016.5675</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>399.37374999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>0.04</v>
       </c>
@@ -21778,15 +21958,15 @@
         <v>3753.95</v>
       </c>
       <c r="P29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1019.05375</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>469.24374999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>0.05</v>
       </c>
@@ -21818,15 +21998,15 @@
         <v>4450.26</v>
       </c>
       <c r="P30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1024.2212500000001</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>556.28250000000003</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>0.1</v>
       </c>
@@ -21858,15 +22038,15 @@
         <v>5550.37</v>
       </c>
       <c r="P31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1017.29625</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>693.79624999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B32" s="5">
         <v>0.5</v>
       </c>
@@ -21898,11 +22078,11 @@
         <v>5808.45</v>
       </c>
       <c r="P32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1014.6825</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>726.05624999999998</v>
       </c>
     </row>
@@ -21938,11 +22118,11 @@
         <v>6192.9</v>
       </c>
       <c r="P33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1016.7887500000001</v>
       </c>
       <c r="Q33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>774.11249999999995</v>
       </c>
     </row>
@@ -21978,11 +22158,11 @@
         <v>6308.84</v>
       </c>
       <c r="P34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1021.95625</v>
       </c>
       <c r="Q34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>788.60500000000002</v>
       </c>
     </row>
@@ -22022,10 +22202,10 @@
       <c r="C37" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D37" s="21" t="s">
+      <c r="D37" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E37" s="21" t="s">
+      <c r="E37" s="18" t="s">
         <v>43</v>
       </c>
       <c r="F37" s="5"/>
@@ -22038,10 +22218,10 @@
       <c r="I37" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J37" s="21" t="s">
+      <c r="J37" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="K37" s="21" t="s">
+      <c r="K37" s="18" t="s">
         <v>45</v>
       </c>
     </row>
@@ -22578,7 +22758,7 @@
       </c>
     </row>
     <row r="50" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="22" t="s">
+      <c r="A50" s="19" t="s">
         <v>25</v>
       </c>
       <c r="B50" s="5" t="s">
@@ -22587,14 +22767,14 @@
       <c r="C50" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D50" s="21" t="s">
+      <c r="D50" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E50" s="21" t="s">
+      <c r="E50" s="18" t="s">
         <v>43</v>
       </c>
       <c r="F50" s="5"/>
-      <c r="G50" s="22" t="s">
+      <c r="G50" s="19" t="s">
         <v>25</v>
       </c>
       <c r="H50" s="5" t="s">
@@ -22603,10 +22783,10 @@
       <c r="I50" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J50" s="21" t="s">
+      <c r="J50" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="K50" s="21" t="s">
+      <c r="K50" s="18" t="s">
         <v>45</v>
       </c>
       <c r="N50" s="12">
@@ -23152,10 +23332,10 @@
       <c r="C62" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D62" s="21" t="s">
+      <c r="D62" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E62" s="21" t="s">
+      <c r="E62" s="18" t="s">
         <v>43</v>
       </c>
       <c r="F62" s="5"/>
@@ -23168,10 +23348,10 @@
       <c r="I62" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J62" s="21" t="s">
+      <c r="J62" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="K62" s="21" t="s">
+      <c r="K62" s="18" t="s">
         <v>45</v>
       </c>
     </row>
@@ -23214,11 +23394,11 @@
         <v>1.0070019531250001</v>
       </c>
       <c r="S63">
-        <f t="shared" ref="S63:T72" si="2">O63/1024</f>
+        <f t="shared" ref="S63:T72" si="6">O63/1024</f>
         <v>1.01577880859375</v>
       </c>
       <c r="T63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.0241723632812501</v>
       </c>
     </row>
@@ -23257,15 +23437,15 @@
         <v>1024.2212500000001</v>
       </c>
       <c r="R64">
-        <f t="shared" ref="R64:R72" si="3">N64/1024</f>
+        <f t="shared" ref="R64:R72" si="7">N64/1024</f>
         <v>1.00335693359375</v>
       </c>
       <c r="S64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.0081201171875001</v>
       </c>
       <c r="T64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.0002160644531251</v>
       </c>
     </row>
@@ -23304,15 +23484,15 @@
         <v>1021.95625</v>
       </c>
       <c r="R65">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.0009106445312499</v>
       </c>
       <c r="S65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.00123291015625</v>
       </c>
       <c r="T65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.99800415039062496</v>
       </c>
     </row>
@@ -23351,15 +23531,15 @@
         <v>1019.3975</v>
       </c>
       <c r="R66">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.99801757812500003</v>
       </c>
       <c r="S66">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.99818725585937496</v>
       </c>
       <c r="T66">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.99550537109375004</v>
       </c>
     </row>
@@ -23398,15 +23578,15 @@
         <v>1019.05375</v>
       </c>
       <c r="R67">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.99648071289062501</v>
       </c>
       <c r="S67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.99604248046874999</v>
       </c>
       <c r="T67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.99516967773437504</v>
       </c>
     </row>
@@ -23445,15 +23625,15 @@
         <v>1017.29625</v>
       </c>
       <c r="R68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.99462768554687497</v>
       </c>
       <c r="S68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.99603149414062497</v>
       </c>
       <c r="T68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.99345336914062499</v>
       </c>
     </row>
@@ -23492,15 +23672,15 @@
         <v>1016.7887500000001</v>
       </c>
       <c r="R69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.99403320312499999</v>
       </c>
       <c r="S69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.99421508789062496</v>
       </c>
       <c r="T69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.99295776367187505</v>
       </c>
     </row>
@@ -23539,15 +23719,15 @@
         <v>1016.5675</v>
       </c>
       <c r="R70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.9930419921875</v>
       </c>
       <c r="S70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.99376586914062504</v>
       </c>
       <c r="T70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.99274169921875</v>
       </c>
     </row>
@@ -23586,15 +23766,15 @@
         <v>1014.6825</v>
       </c>
       <c r="R71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.98863037109374996</v>
       </c>
       <c r="S71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.99302490234374996</v>
       </c>
       <c r="T71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.99090087890625</v>
       </c>
     </row>
@@ -23633,15 +23813,15 @@
         <v>1010.83</v>
       </c>
       <c r="R72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.98838623046874996</v>
       </c>
       <c r="S72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.99224365234375</v>
       </c>
       <c r="T72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.98713867187500004</v>
       </c>
     </row>
@@ -23655,10 +23835,10 @@
       <c r="C74" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D74" s="21" t="s">
+      <c r="D74" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E74" s="21" t="s">
+      <c r="E74" s="18" t="s">
         <v>43</v>
       </c>
       <c r="F74" s="5"/>
@@ -23671,10 +23851,10 @@
       <c r="I74" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J74" s="21" t="s">
+      <c r="J74" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="K74" s="21" t="s">
+      <c r="K74" s="18" t="s">
         <v>45</v>
       </c>
       <c r="N74">

</xml_diff>

<commit_message>
add graph for game BE
</commit_message>
<xml_diff>
--- a/IDBR/excel/resuilt_verify.xlsx
+++ b/IDBR/excel/resuilt_verify.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20377"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20380"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\IDBR\IRDBR\IDBR\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D5647F-B657-40AD-82F5-F8D31DBE941C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B75CF1C-8E23-478E-9B6C-4DD480E336BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-960" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{A13DA03A-EA5C-411C-8535-D1B579D97496}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="48">
   <si>
     <t>alpha</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>SDBR(uncertainty with selection)</t>
+  </si>
+  <si>
+    <t>IDBR(uncertainty)</t>
+  </si>
+  <si>
+    <t>IDBR(uncertainty with selection)</t>
   </si>
 </sst>
 </file>
@@ -12906,7 +12912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E643D7BC-AB9C-4C7D-A150-6AD866B71A01}">
   <dimension ref="A1:AB97"/>
   <sheetViews>
-    <sheetView topLeftCell="E43" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
@@ -18332,10 +18338,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F38528-B6C7-4004-99B1-F08251195C91}">
-  <dimension ref="A1:T84"/>
+  <dimension ref="A1:T97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E3"/>
+      <selection activeCell="D14" sqref="D14:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18349,6 +18355,7 @@
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
     <col min="11" max="11" width="21.85546875" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
@@ -20974,6 +20981,56 @@
       </c>
       <c r="N84">
         <v>0.26582499999999998</v>
+      </c>
+    </row>
+    <row r="88" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C88" s="6">
+        <v>7423150</v>
+      </c>
+    </row>
+    <row r="89" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C89" s="6">
+        <v>7423190</v>
+      </c>
+    </row>
+    <row r="90" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C90" s="6">
+        <v>7657830</v>
+      </c>
+    </row>
+    <row r="91" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C91" s="6">
+        <v>8116030</v>
+      </c>
+    </row>
+    <row r="92" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C92" s="6">
+        <v>8518880</v>
+      </c>
+    </row>
+    <row r="93" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C93" s="6">
+        <v>9734440</v>
+      </c>
+    </row>
+    <row r="94" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C94" s="6">
+        <v>12742300</v>
+      </c>
+    </row>
+    <row r="95" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C95" s="6">
+        <v>13436000</v>
+      </c>
+    </row>
+    <row r="96" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C96" s="6">
+        <v>15532800</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C97" s="6">
+        <v>15831600</v>
       </c>
     </row>
   </sheetData>
@@ -20987,10 +21044,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC5236E-3BC3-4DDA-9C36-963E583DCE32}">
-  <dimension ref="A1:AD84"/>
+  <dimension ref="A1:AD111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E28" workbookViewId="0">
-      <selection activeCell="W22" sqref="W22"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="K106" sqref="G106:K106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21000,10 +21057,11 @@
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" customWidth="1"/>
     <col min="21" max="21" width="15.140625" customWidth="1"/>
     <col min="22" max="22" width="13.42578125" customWidth="1"/>
     <col min="23" max="23" width="11.85546875" customWidth="1"/>
@@ -21123,13 +21181,13 @@
         <v>15</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>14</v>
@@ -21138,13 +21196,13 @@
         <v>15</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N13" s="15">
         <v>7586490</v>
@@ -24386,6 +24444,492 @@
       </c>
       <c r="K84">
         <v>9.3226699999999996E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G88" s="15">
+        <v>7745160</v>
+      </c>
+      <c r="H88" s="15">
+        <v>7586490</v>
+      </c>
+      <c r="I88" s="2">
+        <f>(H88-G88)/G88</f>
+        <v>-2.0486342438374418E-2</v>
+      </c>
+      <c r="J88" s="15">
+        <v>7592260</v>
+      </c>
+      <c r="K88" s="15">
+        <v>7586490</v>
+      </c>
+      <c r="L88" s="2">
+        <f>(K88-J88)/J88</f>
+        <v>-7.5998451054099837E-4</v>
+      </c>
+    </row>
+    <row r="89" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G89" s="15">
+        <v>14497800</v>
+      </c>
+      <c r="H89" s="15">
+        <v>13984300</v>
+      </c>
+      <c r="I89" s="2">
+        <f t="shared" ref="I89:I97" si="8">(H89-G89)/G89</f>
+        <v>-3.5419167046034573E-2</v>
+      </c>
+      <c r="J89" s="15">
+        <v>14434800</v>
+      </c>
+      <c r="K89" s="15">
+        <v>13984300</v>
+      </c>
+      <c r="L89" s="2">
+        <f t="shared" ref="L89:L97" si="9">(K89-J89)/J89</f>
+        <v>-3.1209299747831629E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G90" s="15">
+        <v>20265200</v>
+      </c>
+      <c r="H90" s="15">
+        <v>19148600</v>
+      </c>
+      <c r="I90" s="2">
+        <f t="shared" si="8"/>
+        <v>-5.5099382192132326E-2</v>
+      </c>
+      <c r="J90" s="15">
+        <v>20155700</v>
+      </c>
+      <c r="K90" s="15">
+        <v>19148600</v>
+      </c>
+      <c r="L90" s="2">
+        <f t="shared" si="9"/>
+        <v>-4.9966014576521778E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G91" s="15">
+        <v>25318100</v>
+      </c>
+      <c r="H91" s="15">
+        <v>22386800</v>
+      </c>
+      <c r="I91" s="2">
+        <f t="shared" si="8"/>
+        <v>-0.11577883016498078</v>
+      </c>
+      <c r="J91" s="15">
+        <v>25135800</v>
+      </c>
+      <c r="K91" s="15">
+        <v>22386800</v>
+      </c>
+      <c r="L91" s="2">
+        <f t="shared" si="9"/>
+        <v>-0.1093659242992067</v>
+      </c>
+    </row>
+    <row r="92" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G92" s="15">
+        <v>29512200</v>
+      </c>
+      <c r="H92" s="15">
+        <v>24112700</v>
+      </c>
+      <c r="I92" s="2">
+        <f t="shared" si="8"/>
+        <v>-0.18295823422177948</v>
+      </c>
+      <c r="J92" s="15">
+        <v>29005200</v>
+      </c>
+      <c r="K92" s="15">
+        <v>24112700</v>
+      </c>
+      <c r="L92" s="2">
+        <f t="shared" si="9"/>
+        <v>-0.16867665108325403</v>
+      </c>
+    </row>
+    <row r="93" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G93" s="15">
+        <v>38251300</v>
+      </c>
+      <c r="H93" s="15">
+        <v>25864500</v>
+      </c>
+      <c r="I93" s="2">
+        <f t="shared" si="8"/>
+        <v>-0.32382690261507452</v>
+      </c>
+      <c r="J93" s="15">
+        <v>36920500</v>
+      </c>
+      <c r="K93" s="15">
+        <v>25864500</v>
+      </c>
+      <c r="L93" s="2">
+        <f t="shared" si="9"/>
+        <v>-0.29945423274332689</v>
+      </c>
+    </row>
+    <row r="94" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G94" s="15">
+        <v>48810300</v>
+      </c>
+      <c r="H94" s="15">
+        <v>35751500</v>
+      </c>
+      <c r="I94" s="2">
+        <f t="shared" si="8"/>
+        <v>-0.26754189177284304</v>
+      </c>
+      <c r="J94" s="15">
+        <v>43801500</v>
+      </c>
+      <c r="K94" s="15">
+        <v>35751500</v>
+      </c>
+      <c r="L94" s="2">
+        <f t="shared" si="9"/>
+        <v>-0.18378366037692773</v>
+      </c>
+    </row>
+    <row r="95" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G95" s="15">
+        <v>52748900</v>
+      </c>
+      <c r="H95" s="15">
+        <v>39512600</v>
+      </c>
+      <c r="I95" s="2">
+        <f t="shared" si="8"/>
+        <v>-0.25093035115424206</v>
+      </c>
+      <c r="J95" s="15">
+        <v>46830500</v>
+      </c>
+      <c r="K95" s="15">
+        <v>39512600</v>
+      </c>
+      <c r="L95" s="2">
+        <f t="shared" si="9"/>
+        <v>-0.15626354619318605</v>
+      </c>
+    </row>
+    <row r="96" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G96" s="15">
+        <v>59959500</v>
+      </c>
+      <c r="H96" s="15">
+        <v>45949700</v>
+      </c>
+      <c r="I96" s="2">
+        <f t="shared" si="8"/>
+        <v>-0.23365438337544508</v>
+      </c>
+      <c r="J96" s="15">
+        <v>51608300</v>
+      </c>
+      <c r="K96" s="15">
+        <v>45949700</v>
+      </c>
+      <c r="L96" s="2">
+        <f t="shared" si="9"/>
+        <v>-0.10964515397717034</v>
+      </c>
+    </row>
+    <row r="97" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="G97" s="6">
+        <v>61426900</v>
+      </c>
+      <c r="H97" s="6">
+        <v>47583300</v>
+      </c>
+      <c r="I97" s="2">
+        <f t="shared" si="8"/>
+        <v>-0.22536706231309084</v>
+      </c>
+      <c r="J97" s="6">
+        <v>52562400</v>
+      </c>
+      <c r="K97" s="6">
+        <v>47583300</v>
+      </c>
+      <c r="L97" s="2">
+        <f t="shared" si="9"/>
+        <v>-9.4727409707319299E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="I98" s="2">
+        <f>AVERAGE(I88:I97)</f>
+        <v>-0.17110625472939972</v>
+      </c>
+      <c r="L98" s="2">
+        <f>AVERAGE(L88:L97)</f>
+        <v>-0.12038518772152855</v>
+      </c>
+    </row>
+    <row r="101" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F101" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="G101" s="12">
+        <v>0</v>
+      </c>
+      <c r="H101" s="12">
+        <v>0</v>
+      </c>
+      <c r="I101" s="2">
+        <v>0</v>
+      </c>
+      <c r="J101" s="12">
+        <v>0</v>
+      </c>
+      <c r="K101" s="12">
+        <v>0</v>
+      </c>
+      <c r="L101" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F102" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="G102" s="12">
+        <v>0</v>
+      </c>
+      <c r="H102" s="12">
+        <v>0</v>
+      </c>
+      <c r="I102" s="2">
+        <v>0</v>
+      </c>
+      <c r="J102" s="12">
+        <v>0</v>
+      </c>
+      <c r="K102" s="12">
+        <v>0</v>
+      </c>
+      <c r="L102" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F103" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="G103" s="12">
+        <v>3.1053100000000001E-4</v>
+      </c>
+      <c r="H103" s="12">
+        <v>3.22785E-3</v>
+      </c>
+      <c r="I103" s="2">
+        <f t="shared" ref="I102:I110" si="10">(H103-G103)/G103</f>
+        <v>9.3946143863253582</v>
+      </c>
+      <c r="J103" s="12">
+        <v>1.77567E-4</v>
+      </c>
+      <c r="K103" s="12">
+        <v>3.22785E-3</v>
+      </c>
+      <c r="L103" s="2">
+        <f t="shared" ref="L102:L110" si="11">(K103-J103)/J103</f>
+        <v>17.178208788795214</v>
+      </c>
+    </row>
+    <row r="104" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F104" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="G104" s="12">
+        <v>2.5625399999999999E-3</v>
+      </c>
+      <c r="H104" s="12">
+        <v>3.0062599999999998E-2</v>
+      </c>
+      <c r="I104" s="2">
+        <f t="shared" si="10"/>
+        <v>10.731563214622991</v>
+      </c>
+      <c r="J104" s="12">
+        <v>3.4576400000000001E-3</v>
+      </c>
+      <c r="K104" s="12">
+        <v>3.0062599999999998E-2</v>
+      </c>
+      <c r="L104" s="2">
+        <f t="shared" si="11"/>
+        <v>7.6945430987610033</v>
+      </c>
+    </row>
+    <row r="105" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F105" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="G105" s="12">
+        <v>1.6429200000000001E-2</v>
+      </c>
+      <c r="H105" s="12">
+        <v>0.10780000000000001</v>
+      </c>
+      <c r="I105" s="2">
+        <f t="shared" si="10"/>
+        <v>5.5614880821951154</v>
+      </c>
+      <c r="J105" s="12">
+        <v>2.2094099999999998E-2</v>
+      </c>
+      <c r="K105" s="12">
+        <v>0.10780000000000001</v>
+      </c>
+      <c r="L105" s="2">
+        <f t="shared" si="11"/>
+        <v>3.8791306276336219</v>
+      </c>
+    </row>
+    <row r="106" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F106" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G106" s="12">
+        <v>0.29509600000000002</v>
+      </c>
+      <c r="H106" s="12">
+        <v>0.47873199999999999</v>
+      </c>
+      <c r="I106" s="2">
+        <f t="shared" si="10"/>
+        <v>0.62229240653888884</v>
+      </c>
+      <c r="J106" s="12">
+        <v>0.31213299999999999</v>
+      </c>
+      <c r="K106" s="12">
+        <v>0.47873199999999999</v>
+      </c>
+      <c r="L106" s="2">
+        <f t="shared" si="11"/>
+        <v>0.5337436285173307</v>
+      </c>
+    </row>
+    <row r="107" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F107" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G107" s="12">
+        <v>0.81214699999999995</v>
+      </c>
+      <c r="H107" s="12">
+        <v>0.84668600000000005</v>
+      </c>
+      <c r="I107" s="2">
+        <f t="shared" si="10"/>
+        <v>4.2528015248471149E-2</v>
+      </c>
+      <c r="J107" s="12">
+        <v>0.83248800000000001</v>
+      </c>
+      <c r="K107" s="12">
+        <v>0.84668600000000005</v>
+      </c>
+      <c r="L107" s="2">
+        <f t="shared" si="11"/>
+        <v>1.7054900491058182E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F108" s="5">
+        <v>1</v>
+      </c>
+      <c r="G108" s="12">
+        <v>0.896783</v>
+      </c>
+      <c r="H108" s="12">
+        <v>0.91367500000000001</v>
+      </c>
+      <c r="I108" s="2">
+        <f t="shared" si="10"/>
+        <v>1.8836217903327804E-2</v>
+      </c>
+      <c r="J108" s="12">
+        <v>0.90895599999999999</v>
+      </c>
+      <c r="K108" s="12">
+        <v>0.91367500000000001</v>
+      </c>
+      <c r="L108" s="2">
+        <f t="shared" si="11"/>
+        <v>5.1916704438939058E-3</v>
+      </c>
+    </row>
+    <row r="109" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F109" s="5">
+        <v>5</v>
+      </c>
+      <c r="G109" s="12">
+        <v>0.97603499999999999</v>
+      </c>
+      <c r="H109" s="12">
+        <v>0.97940899999999997</v>
+      </c>
+      <c r="I109" s="2">
+        <f t="shared" si="10"/>
+        <v>3.4568432484490702E-3</v>
+      </c>
+      <c r="J109" s="12">
+        <v>0.97953000000000001</v>
+      </c>
+      <c r="K109" s="12">
+        <v>0.97940899999999997</v>
+      </c>
+      <c r="L109" s="2">
+        <f t="shared" si="11"/>
+        <v>-1.2352863107820868E-4</v>
+      </c>
+    </row>
+    <row r="110" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F110" s="5">
+        <v>10</v>
+      </c>
+      <c r="G110" s="12">
+        <v>0.98763800000000002</v>
+      </c>
+      <c r="H110" s="12">
+        <v>0.989317</v>
+      </c>
+      <c r="I110" s="2">
+        <f t="shared" si="10"/>
+        <v>1.7000155927576561E-3</v>
+      </c>
+      <c r="J110" s="12">
+        <v>0.98952399999999996</v>
+      </c>
+      <c r="K110" s="12">
+        <v>0.989317</v>
+      </c>
+      <c r="L110" s="2">
+        <f t="shared" si="11"/>
+        <v>-2.0919149004971807E-4</v>
+      </c>
+    </row>
+    <row r="111" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="I111" s="2">
+        <f>AVERAGE(I101:I110)</f>
+        <v>2.6376479181675361</v>
+      </c>
+      <c r="L111" s="2">
+        <f>AVERAGE(L101:L110)</f>
+        <v>2.930753999452099</v>
       </c>
     </row>
   </sheetData>

</xml_diff>